<commit_message>
danh sach nguon nhap, xử lý thanh lý thuoc bên tram y te
</commit_message>
<xml_diff>
--- a/storage/app/public/data/danhsachthuoc.xlsx
+++ b/storage/app/public/data/danhsachthuoc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2138" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="429">
   <si>
     <t>Tên thuốc</t>
   </si>
@@ -1717,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="A200" sqref="A200:K305"/>
+    <sheetView tabSelected="1" topLeftCell="C199" workbookViewId="0">
+      <selection activeCell="N98" sqref="N98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2458,7 +2458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>109</v>
       </c>
@@ -8689,7 +8689,9 @@
       </c>
     </row>
     <row r="200" spans="1:11" ht="51" x14ac:dyDescent="0.3">
-      <c r="A200" s="5"/>
+      <c r="A200" s="5" t="s">
+        <v>399</v>
+      </c>
       <c r="B200" s="5">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
--chức năng phân loại thuốc
</commit_message>
<xml_diff>
--- a/storage/app/public/data/danhsachthuoc.xlsx
+++ b/storage/app/public/data/danhsachthuoc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2140" uniqueCount="430">
   <si>
     <t>Tên thuốc</t>
   </si>
@@ -1311,6 +1311,9 @@
   </si>
   <si>
     <t>Công ty TNHH B.Braun Việt Nam</t>
+  </si>
+  <si>
+    <t>Tên phân loại</t>
   </si>
 </sst>
 </file>
@@ -1321,7 +1324,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1351,6 +1354,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1410,7 +1419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1434,6 +1443,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1715,15 +1725,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K305"/>
+  <dimension ref="A1:L305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C199" workbookViewId="0">
-      <selection activeCell="N98" sqref="N98"/>
+    <sheetView tabSelected="1" topLeftCell="A301" workbookViewId="0">
+      <selection activeCell="O304" sqref="O304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1757,8 +1767,11 @@
       <c r="K1" s="1" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L1" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1792,8 +1805,11 @@
       <c r="K2" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L2" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1827,8 +1843,11 @@
       <c r="K3" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L3" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -1862,8 +1881,11 @@
       <c r="K4" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L4" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -1897,8 +1919,11 @@
       <c r="K5" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
@@ -1932,8 +1957,11 @@
       <c r="K6" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L6" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>40</v>
       </c>
@@ -1967,8 +1995,11 @@
       <c r="K7" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L7" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>45</v>
       </c>
@@ -2002,8 +2033,11 @@
       <c r="K8" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L8" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>49</v>
       </c>
@@ -2037,8 +2071,11 @@
       <c r="K9" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L9" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>52</v>
       </c>
@@ -2072,8 +2109,11 @@
       <c r="K10" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="132.6" x14ac:dyDescent="0.3">
+      <c r="L10" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>56</v>
       </c>
@@ -2107,8 +2147,11 @@
       <c r="K11" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L11" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>61</v>
       </c>
@@ -2142,8 +2185,11 @@
       <c r="K12" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L12" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>66</v>
       </c>
@@ -2177,8 +2223,11 @@
       <c r="K13" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L13" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>72</v>
       </c>
@@ -2212,8 +2261,11 @@
       <c r="K14" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L14" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>78</v>
       </c>
@@ -2247,8 +2299,11 @@
       <c r="K15" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L15" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>82</v>
       </c>
@@ -2282,8 +2337,11 @@
       <c r="K16" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L16" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>85</v>
       </c>
@@ -2317,8 +2375,11 @@
       <c r="K17" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="71.400000000000006" x14ac:dyDescent="0.3">
+      <c r="L17" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="71.400000000000006" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>90</v>
       </c>
@@ -2352,8 +2413,11 @@
       <c r="K18" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L18" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>93</v>
       </c>
@@ -2387,8 +2451,11 @@
       <c r="K19" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L19" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>100</v>
       </c>
@@ -2422,8 +2489,11 @@
       <c r="K20" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L20" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>103</v>
       </c>
@@ -2457,8 +2527,11 @@
       <c r="K21" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L21" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>109</v>
       </c>
@@ -2492,8 +2565,11 @@
       <c r="K22" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L22" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>112</v>
       </c>
@@ -2527,8 +2603,11 @@
       <c r="K23" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L23" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>117</v>
       </c>
@@ -2562,8 +2641,11 @@
       <c r="K24" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L24" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>123</v>
       </c>
@@ -2597,8 +2679,11 @@
       <c r="K25" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L25" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>126</v>
       </c>
@@ -2632,8 +2717,11 @@
       <c r="K26" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L26" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>132</v>
       </c>
@@ -2667,8 +2755,11 @@
       <c r="K27" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L27" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>137</v>
       </c>
@@ -2702,8 +2793,11 @@
       <c r="K28" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L28" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>141</v>
       </c>
@@ -2737,8 +2831,11 @@
       <c r="K29" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L29" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>145</v>
       </c>
@@ -2772,8 +2869,11 @@
       <c r="K30" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L30" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>151</v>
       </c>
@@ -2807,8 +2907,11 @@
       <c r="K31" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L31" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>153</v>
       </c>
@@ -2842,8 +2945,11 @@
       <c r="K32" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L32" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>156</v>
       </c>
@@ -2877,8 +2983,11 @@
       <c r="K33" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L33" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>162</v>
       </c>
@@ -2912,8 +3021,11 @@
       <c r="K34" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" ht="71.400000000000006" x14ac:dyDescent="0.3">
+      <c r="L34" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="71.400000000000006" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>165</v>
       </c>
@@ -2947,8 +3059,11 @@
       <c r="K35" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L35" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>171</v>
       </c>
@@ -2982,8 +3097,11 @@
       <c r="K36" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L36" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>175</v>
       </c>
@@ -3017,8 +3135,11 @@
       <c r="K37" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L37" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>182</v>
       </c>
@@ -3052,8 +3173,11 @@
       <c r="K38" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L38" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>182</v>
       </c>
@@ -3087,8 +3211,11 @@
       <c r="K39" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L39" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>189</v>
       </c>
@@ -3122,8 +3249,11 @@
       <c r="K40" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" ht="91.8" x14ac:dyDescent="0.3">
+      <c r="L40" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>193</v>
       </c>
@@ -3157,8 +3287,11 @@
       <c r="K41" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L41" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>196</v>
       </c>
@@ -3192,8 +3325,11 @@
       <c r="K42" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L42" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>199</v>
       </c>
@@ -3227,8 +3363,11 @@
       <c r="K43" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L43" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>203</v>
       </c>
@@ -3262,8 +3401,11 @@
       <c r="K44" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L44" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>207</v>
       </c>
@@ -3297,8 +3439,11 @@
       <c r="K45" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" ht="91.8" x14ac:dyDescent="0.3">
+      <c r="L45" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>209</v>
       </c>
@@ -3332,8 +3477,11 @@
       <c r="K46" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L46" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>210</v>
       </c>
@@ -3367,8 +3515,11 @@
       <c r="K47" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L47" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>212</v>
       </c>
@@ -3402,8 +3553,11 @@
       <c r="K48" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L48" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>215</v>
       </c>
@@ -3437,8 +3591,11 @@
       <c r="K49" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L49" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>217</v>
       </c>
@@ -3472,8 +3629,11 @@
       <c r="K50" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L50" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>218</v>
       </c>
@@ -3507,8 +3667,11 @@
       <c r="K51" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L51" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>225</v>
       </c>
@@ -3542,8 +3705,11 @@
       <c r="K52" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L52" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>227</v>
       </c>
@@ -3577,8 +3743,11 @@
       <c r="K53" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L53" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>232</v>
       </c>
@@ -3612,8 +3781,11 @@
       <c r="K54" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L54" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>238</v>
       </c>
@@ -3647,8 +3819,11 @@
       <c r="K55" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L55" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>243</v>
       </c>
@@ -3682,8 +3857,11 @@
       <c r="K56" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L56" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>249</v>
       </c>
@@ -3717,8 +3895,11 @@
       <c r="K57" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L57" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>250</v>
       </c>
@@ -3752,8 +3933,11 @@
       <c r="K58" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L58" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>255</v>
       </c>
@@ -3787,8 +3971,11 @@
       <c r="K59" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L59" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>260</v>
       </c>
@@ -3822,8 +4009,11 @@
       <c r="K60" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L60" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>260</v>
       </c>
@@ -3857,8 +4047,11 @@
       <c r="K61" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L61" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>260</v>
       </c>
@@ -3892,8 +4085,11 @@
       <c r="K62" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L62" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>267</v>
       </c>
@@ -3927,8 +4123,11 @@
       <c r="K63" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L63" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>270</v>
       </c>
@@ -3962,8 +4161,11 @@
       <c r="K64" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L64" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>274</v>
       </c>
@@ -3997,8 +4199,11 @@
       <c r="K65" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L65" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>278</v>
       </c>
@@ -4032,8 +4237,11 @@
       <c r="K66" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L66" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>281</v>
       </c>
@@ -4067,8 +4275,11 @@
       <c r="K67" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L67" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>285</v>
       </c>
@@ -4102,8 +4313,11 @@
       <c r="K68" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L68" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>290</v>
       </c>
@@ -4137,8 +4351,11 @@
       <c r="K69" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L69" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>293</v>
       </c>
@@ -4172,8 +4389,11 @@
       <c r="K70" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L70" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>298</v>
       </c>
@@ -4207,8 +4427,11 @@
       <c r="K71" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L71" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>301</v>
       </c>
@@ -4242,8 +4465,11 @@
       <c r="K72" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L72" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>307</v>
       </c>
@@ -4277,8 +4503,11 @@
       <c r="K73" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L73" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>312</v>
       </c>
@@ -4312,8 +4541,11 @@
       <c r="K74" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L74" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>316</v>
       </c>
@@ -4347,8 +4579,11 @@
       <c r="K75" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L75" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>318</v>
       </c>
@@ -4382,8 +4617,11 @@
       <c r="K76" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L76" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>321</v>
       </c>
@@ -4417,8 +4655,11 @@
       <c r="K77" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L77" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>325</v>
       </c>
@@ -4452,8 +4693,11 @@
       <c r="K78" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L78" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>329</v>
       </c>
@@ -4487,8 +4731,11 @@
       <c r="K79" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L79" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>331</v>
       </c>
@@ -4522,8 +4769,11 @@
       <c r="K80" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L80" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>336</v>
       </c>
@@ -4557,8 +4807,11 @@
       <c r="K81" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L81" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>339</v>
       </c>
@@ -4592,8 +4845,11 @@
       <c r="K82" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L82" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>343</v>
       </c>
@@ -4627,8 +4883,11 @@
       <c r="K83" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L83" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>345</v>
       </c>
@@ -4662,8 +4921,11 @@
       <c r="K84" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L84" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>347</v>
       </c>
@@ -4697,8 +4959,11 @@
       <c r="K85" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L85" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>348</v>
       </c>
@@ -4732,8 +4997,11 @@
       <c r="K86" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L86" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>353</v>
       </c>
@@ -4767,8 +5035,11 @@
       <c r="K87" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L87" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>355</v>
       </c>
@@ -4802,8 +5073,11 @@
       <c r="K88" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L88" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>358</v>
       </c>
@@ -4837,8 +5111,11 @@
       <c r="K89" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L89" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>361</v>
       </c>
@@ -4872,8 +5149,11 @@
       <c r="K90" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" ht="81.599999999999994" x14ac:dyDescent="0.3">
+      <c r="L90" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>363</v>
       </c>
@@ -4907,8 +5187,11 @@
       <c r="K91" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L91" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>369</v>
       </c>
@@ -4942,8 +5225,11 @@
       <c r="K92" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L92" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>373</v>
       </c>
@@ -4977,8 +5263,11 @@
       <c r="K93" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L93" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>376</v>
       </c>
@@ -5012,8 +5301,11 @@
       <c r="K94" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L94" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>379</v>
       </c>
@@ -5047,8 +5339,11 @@
       <c r="K95" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" ht="91.8" x14ac:dyDescent="0.3">
+      <c r="L95" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>383</v>
       </c>
@@ -5082,8 +5377,11 @@
       <c r="K96" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L96" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>385</v>
       </c>
@@ -5117,8 +5415,11 @@
       <c r="K97" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" ht="81.599999999999994" x14ac:dyDescent="0.3">
+      <c r="L97" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>389</v>
       </c>
@@ -5152,8 +5453,11 @@
       <c r="K98" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L98" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>394</v>
       </c>
@@ -5187,8 +5491,11 @@
       <c r="K99" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L99" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>399</v>
       </c>
@@ -5222,8 +5529,11 @@
       <c r="K100" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L100" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>10</v>
       </c>
@@ -5257,8 +5567,9 @@
       <c r="K101" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L101" s="9"/>
+    </row>
+    <row r="102" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>17</v>
       </c>
@@ -5292,8 +5603,9 @@
       <c r="K102" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L102" s="9"/>
+    </row>
+    <row r="103" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>23</v>
       </c>
@@ -5327,8 +5639,9 @@
       <c r="K103" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L103" s="9"/>
+    </row>
+    <row r="104" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>27</v>
       </c>
@@ -5362,8 +5675,9 @@
       <c r="K104" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L104" s="9"/>
+    </row>
+    <row r="105" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>34</v>
       </c>
@@ -5397,8 +5711,9 @@
       <c r="K105" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L105" s="9"/>
+    </row>
+    <row r="106" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>40</v>
       </c>
@@ -5432,8 +5747,9 @@
       <c r="K106" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L106" s="9"/>
+    </row>
+    <row r="107" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>45</v>
       </c>
@@ -5467,8 +5783,9 @@
       <c r="K107" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L107" s="9"/>
+    </row>
+    <row r="108" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>49</v>
       </c>
@@ -5502,8 +5819,9 @@
       <c r="K108" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L108" s="9"/>
+    </row>
+    <row r="109" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>52</v>
       </c>
@@ -5537,8 +5855,9 @@
       <c r="K109" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" ht="132.6" x14ac:dyDescent="0.3">
+      <c r="L109" s="9"/>
+    </row>
+    <row r="110" spans="1:12" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>56</v>
       </c>
@@ -5572,8 +5891,9 @@
       <c r="K110" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L110" s="9"/>
+    </row>
+    <row r="111" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>61</v>
       </c>
@@ -5607,8 +5927,9 @@
       <c r="K111" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L111" s="9"/>
+    </row>
+    <row r="112" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>66</v>
       </c>
@@ -5642,8 +5963,9 @@
       <c r="K112" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L112" s="9"/>
+    </row>
+    <row r="113" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>72</v>
       </c>
@@ -5677,8 +5999,9 @@
       <c r="K113" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L113" s="9"/>
+    </row>
+    <row r="114" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>78</v>
       </c>
@@ -5712,8 +6035,9 @@
       <c r="K114" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L114" s="9"/>
+    </row>
+    <row r="115" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>82</v>
       </c>
@@ -5747,8 +6071,9 @@
       <c r="K115" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L115" s="9"/>
+    </row>
+    <row r="116" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>85</v>
       </c>
@@ -5782,8 +6107,9 @@
       <c r="K116" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" ht="71.400000000000006" x14ac:dyDescent="0.3">
+      <c r="L116" s="9"/>
+    </row>
+    <row r="117" spans="1:12" ht="71.400000000000006" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>90</v>
       </c>
@@ -5817,8 +6143,9 @@
       <c r="K117" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L117" s="9"/>
+    </row>
+    <row r="118" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>93</v>
       </c>
@@ -5852,8 +6179,9 @@
       <c r="K118" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L118" s="9"/>
+    </row>
+    <row r="119" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>100</v>
       </c>
@@ -5887,8 +6215,9 @@
       <c r="K119" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L119" s="9"/>
+    </row>
+    <row r="120" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>103</v>
       </c>
@@ -5922,8 +6251,9 @@
       <c r="K120" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L120" s="9"/>
+    </row>
+    <row r="121" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>109</v>
       </c>
@@ -5957,8 +6287,9 @@
       <c r="K121" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L121" s="9"/>
+    </row>
+    <row r="122" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>112</v>
       </c>
@@ -5992,8 +6323,9 @@
       <c r="K122" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L122" s="9"/>
+    </row>
+    <row r="123" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>117</v>
       </c>
@@ -6027,8 +6359,9 @@
       <c r="K123" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L123" s="9"/>
+    </row>
+    <row r="124" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>123</v>
       </c>
@@ -6062,8 +6395,9 @@
       <c r="K124" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L124" s="9"/>
+    </row>
+    <row r="125" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>126</v>
       </c>
@@ -6097,8 +6431,9 @@
       <c r="K125" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L125" s="9"/>
+    </row>
+    <row r="126" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>132</v>
       </c>
@@ -6132,8 +6467,9 @@
       <c r="K126" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L126" s="9"/>
+    </row>
+    <row r="127" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>137</v>
       </c>
@@ -6167,8 +6503,9 @@
       <c r="K127" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L127" s="9"/>
+    </row>
+    <row r="128" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>141</v>
       </c>
@@ -6202,8 +6539,9 @@
       <c r="K128" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L128" s="9"/>
+    </row>
+    <row r="129" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>145</v>
       </c>
@@ -6237,8 +6575,9 @@
       <c r="K129" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L129" s="9"/>
+    </row>
+    <row r="130" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>151</v>
       </c>
@@ -6272,8 +6611,9 @@
       <c r="K130" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L130" s="9"/>
+    </row>
+    <row r="131" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>153</v>
       </c>
@@ -6307,8 +6647,9 @@
       <c r="K131" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L131" s="9"/>
+    </row>
+    <row r="132" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>156</v>
       </c>
@@ -6342,8 +6683,9 @@
       <c r="K132" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L132" s="9"/>
+    </row>
+    <row r="133" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>162</v>
       </c>
@@ -6377,8 +6719,9 @@
       <c r="K133" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" ht="71.400000000000006" x14ac:dyDescent="0.3">
+      <c r="L133" s="9"/>
+    </row>
+    <row r="134" spans="1:12" ht="71.400000000000006" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>165</v>
       </c>
@@ -6412,8 +6755,9 @@
       <c r="K134" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L134" s="9"/>
+    </row>
+    <row r="135" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>171</v>
       </c>
@@ -6447,8 +6791,9 @@
       <c r="K135" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L135" s="9"/>
+    </row>
+    <row r="136" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>175</v>
       </c>
@@ -6482,8 +6827,9 @@
       <c r="K136" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L136" s="9"/>
+    </row>
+    <row r="137" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>182</v>
       </c>
@@ -6517,8 +6863,9 @@
       <c r="K137" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L137" s="9"/>
+    </row>
+    <row r="138" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>182</v>
       </c>
@@ -6552,8 +6899,9 @@
       <c r="K138" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L138" s="9"/>
+    </row>
+    <row r="139" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>189</v>
       </c>
@@ -6587,8 +6935,9 @@
       <c r="K139" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" ht="91.8" x14ac:dyDescent="0.3">
+      <c r="L139" s="9"/>
+    </row>
+    <row r="140" spans="1:12" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>193</v>
       </c>
@@ -6622,8 +6971,9 @@
       <c r="K140" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L140" s="9"/>
+    </row>
+    <row r="141" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>196</v>
       </c>
@@ -6657,8 +7007,9 @@
       <c r="K141" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L141" s="9"/>
+    </row>
+    <row r="142" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>199</v>
       </c>
@@ -6692,8 +7043,9 @@
       <c r="K142" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L142" s="9"/>
+    </row>
+    <row r="143" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>203</v>
       </c>
@@ -6727,8 +7079,9 @@
       <c r="K143" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L143" s="9"/>
+    </row>
+    <row r="144" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>207</v>
       </c>
@@ -6762,8 +7115,9 @@
       <c r="K144" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" ht="91.8" x14ac:dyDescent="0.3">
+      <c r="L144" s="9"/>
+    </row>
+    <row r="145" spans="1:12" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>209</v>
       </c>
@@ -6797,8 +7151,9 @@
       <c r="K145" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L145" s="9"/>
+    </row>
+    <row r="146" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>210</v>
       </c>
@@ -6832,8 +7187,9 @@
       <c r="K146" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L146" s="9"/>
+    </row>
+    <row r="147" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>212</v>
       </c>
@@ -6867,8 +7223,9 @@
       <c r="K147" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="148" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L147" s="9"/>
+    </row>
+    <row r="148" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>215</v>
       </c>
@@ -6902,8 +7259,9 @@
       <c r="K148" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="149" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L148" s="9"/>
+    </row>
+    <row r="149" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>217</v>
       </c>
@@ -6937,8 +7295,9 @@
       <c r="K149" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="150" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L149" s="9"/>
+    </row>
+    <row r="150" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>218</v>
       </c>
@@ -6972,8 +7331,9 @@
       <c r="K150" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L150" s="9"/>
+    </row>
+    <row r="151" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>225</v>
       </c>
@@ -7007,8 +7367,9 @@
       <c r="K151" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="152" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L151" s="9"/>
+    </row>
+    <row r="152" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>227</v>
       </c>
@@ -7042,8 +7403,9 @@
       <c r="K152" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L152" s="9"/>
+    </row>
+    <row r="153" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>232</v>
       </c>
@@ -7077,8 +7439,9 @@
       <c r="K153" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L153" s="9"/>
+    </row>
+    <row r="154" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>238</v>
       </c>
@@ -7112,8 +7475,9 @@
       <c r="K154" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="155" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L154" s="9"/>
+    </row>
+    <row r="155" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>243</v>
       </c>
@@ -7147,8 +7511,9 @@
       <c r="K155" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="156" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L155" s="9"/>
+    </row>
+    <row r="156" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>249</v>
       </c>
@@ -7182,8 +7547,9 @@
       <c r="K156" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L156" s="9"/>
+    </row>
+    <row r="157" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>250</v>
       </c>
@@ -7217,8 +7583,9 @@
       <c r="K157" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="158" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L157" s="9"/>
+    </row>
+    <row r="158" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>255</v>
       </c>
@@ -7252,8 +7619,9 @@
       <c r="K158" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="159" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L158" s="9"/>
+    </row>
+    <row r="159" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>260</v>
       </c>
@@ -7287,8 +7655,9 @@
       <c r="K159" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="160" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L159" s="9"/>
+    </row>
+    <row r="160" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
         <v>260</v>
       </c>
@@ -7322,8 +7691,9 @@
       <c r="K160" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L160" s="9"/>
+    </row>
+    <row r="161" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>260</v>
       </c>
@@ -7357,8 +7727,9 @@
       <c r="K161" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="162" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L161" s="9"/>
+    </row>
+    <row r="162" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>267</v>
       </c>
@@ -7392,8 +7763,9 @@
       <c r="K162" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="163" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L162" s="9"/>
+    </row>
+    <row r="163" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
         <v>270</v>
       </c>
@@ -7427,8 +7799,9 @@
       <c r="K163" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L163" s="9"/>
+    </row>
+    <row r="164" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
         <v>274</v>
       </c>
@@ -7462,8 +7835,9 @@
       <c r="K164" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="165" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L164" s="9"/>
+    </row>
+    <row r="165" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>278</v>
       </c>
@@ -7497,8 +7871,9 @@
       <c r="K165" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="166" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L165" s="9"/>
+    </row>
+    <row r="166" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>281</v>
       </c>
@@ -7532,8 +7907,9 @@
       <c r="K166" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="167" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L166" s="9"/>
+    </row>
+    <row r="167" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>285</v>
       </c>
@@ -7567,8 +7943,9 @@
       <c r="K167" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="168" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L167" s="9"/>
+    </row>
+    <row r="168" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>290</v>
       </c>
@@ -7602,8 +7979,9 @@
       <c r="K168" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="169" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L168" s="9"/>
+    </row>
+    <row r="169" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>293</v>
       </c>
@@ -7637,8 +8015,9 @@
       <c r="K169" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="170" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L169" s="9"/>
+    </row>
+    <row r="170" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
         <v>298</v>
       </c>
@@ -7672,8 +8051,9 @@
       <c r="K170" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="171" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L170" s="9"/>
+    </row>
+    <row r="171" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>301</v>
       </c>
@@ -7707,8 +8087,9 @@
       <c r="K171" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="172" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L171" s="9"/>
+    </row>
+    <row r="172" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>307</v>
       </c>
@@ -7742,8 +8123,9 @@
       <c r="K172" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="173" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L172" s="9"/>
+    </row>
+    <row r="173" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
         <v>312</v>
       </c>
@@ -7777,8 +8159,9 @@
       <c r="K173" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="174" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L173" s="9"/>
+    </row>
+    <row r="174" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
         <v>316</v>
       </c>
@@ -7812,8 +8195,9 @@
       <c r="K174" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="175" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L174" s="9"/>
+    </row>
+    <row r="175" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
         <v>318</v>
       </c>
@@ -7847,8 +8231,9 @@
       <c r="K175" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="176" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L175" s="9"/>
+    </row>
+    <row r="176" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
         <v>321</v>
       </c>
@@ -7882,8 +8267,9 @@
       <c r="K176" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="177" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L176" s="9"/>
+    </row>
+    <row r="177" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
         <v>325</v>
       </c>
@@ -7917,8 +8303,9 @@
       <c r="K177" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="178" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L177" s="9"/>
+    </row>
+    <row r="178" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>329</v>
       </c>
@@ -7952,8 +8339,9 @@
       <c r="K178" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="179" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L178" s="9"/>
+    </row>
+    <row r="179" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
         <v>331</v>
       </c>
@@ -7987,8 +8375,9 @@
       <c r="K179" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="180" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L179" s="9"/>
+    </row>
+    <row r="180" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
         <v>336</v>
       </c>
@@ -8022,8 +8411,9 @@
       <c r="K180" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="181" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L180" s="9"/>
+    </row>
+    <row r="181" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
         <v>339</v>
       </c>
@@ -8057,8 +8447,9 @@
       <c r="K181" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="182" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L181" s="9"/>
+    </row>
+    <row r="182" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A182" s="5" t="s">
         <v>343</v>
       </c>
@@ -8092,8 +8483,9 @@
       <c r="K182" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="183" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L182" s="9"/>
+    </row>
+    <row r="183" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
         <v>345</v>
       </c>
@@ -8127,8 +8519,9 @@
       <c r="K183" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="184" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L183" s="9"/>
+    </row>
+    <row r="184" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
         <v>347</v>
       </c>
@@ -8162,8 +8555,9 @@
       <c r="K184" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="185" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L184" s="9"/>
+    </row>
+    <row r="185" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A185" s="5" t="s">
         <v>348</v>
       </c>
@@ -8197,8 +8591,9 @@
       <c r="K185" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="186" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L185" s="9"/>
+    </row>
+    <row r="186" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
         <v>353</v>
       </c>
@@ -8232,8 +8627,9 @@
       <c r="K186" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="187" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L186" s="9"/>
+    </row>
+    <row r="187" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
         <v>355</v>
       </c>
@@ -8267,8 +8663,9 @@
       <c r="K187" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="188" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L187" s="9"/>
+    </row>
+    <row r="188" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
         <v>358</v>
       </c>
@@ -8302,8 +8699,9 @@
       <c r="K188" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="189" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L188" s="9"/>
+    </row>
+    <row r="189" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
         <v>361</v>
       </c>
@@ -8337,8 +8735,9 @@
       <c r="K189" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="190" spans="1:11" ht="81.599999999999994" x14ac:dyDescent="0.3">
+      <c r="L189" s="9"/>
+    </row>
+    <row r="190" spans="1:12" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A190" s="5" t="s">
         <v>363</v>
       </c>
@@ -8372,8 +8771,9 @@
       <c r="K190" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="191" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L190" s="9"/>
+    </row>
+    <row r="191" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A191" s="5" t="s">
         <v>369</v>
       </c>
@@ -8407,8 +8807,9 @@
       <c r="K191" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="192" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L191" s="9"/>
+    </row>
+    <row r="192" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A192" s="5" t="s">
         <v>373</v>
       </c>
@@ -8442,8 +8843,9 @@
       <c r="K192" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="193" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L192" s="9"/>
+    </row>
+    <row r="193" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
         <v>376</v>
       </c>
@@ -8477,8 +8879,9 @@
       <c r="K193" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="194" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L193" s="9"/>
+    </row>
+    <row r="194" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A194" s="5" t="s">
         <v>379</v>
       </c>
@@ -8512,8 +8915,9 @@
       <c r="K194" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="195" spans="1:11" ht="91.8" x14ac:dyDescent="0.3">
+      <c r="L194" s="9"/>
+    </row>
+    <row r="195" spans="1:12" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A195" s="5" t="s">
         <v>383</v>
       </c>
@@ -8547,8 +8951,9 @@
       <c r="K195" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="196" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L195" s="9"/>
+    </row>
+    <row r="196" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A196" s="5" t="s">
         <v>385</v>
       </c>
@@ -8582,8 +8987,9 @@
       <c r="K196" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="197" spans="1:11" ht="81.599999999999994" x14ac:dyDescent="0.3">
+      <c r="L196" s="9"/>
+    </row>
+    <row r="197" spans="1:12" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A197" s="5" t="s">
         <v>389</v>
       </c>
@@ -8617,8 +9023,9 @@
       <c r="K197" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="198" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L197" s="9"/>
+    </row>
+    <row r="198" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A198" s="5" t="s">
         <v>394</v>
       </c>
@@ -8652,8 +9059,9 @@
       <c r="K198" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="199" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L198" s="9"/>
+    </row>
+    <row r="199" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A199" s="5" t="s">
         <v>399</v>
       </c>
@@ -8687,8 +9095,9 @@
       <c r="K199" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="200" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L199" s="9"/>
+    </row>
+    <row r="200" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A200" s="5" t="s">
         <v>399</v>
       </c>
@@ -8722,8 +9131,11 @@
       <c r="K200" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="201" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L200" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A201" s="5" t="s">
         <v>17</v>
       </c>
@@ -8757,8 +9169,11 @@
       <c r="K201" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="202" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L201" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A202" s="5" t="s">
         <v>23</v>
       </c>
@@ -8792,8 +9207,11 @@
       <c r="K202" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="203" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L202" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A203" s="5" t="s">
         <v>27</v>
       </c>
@@ -8827,8 +9245,11 @@
       <c r="K203" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="204" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L203" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A204" s="5" t="s">
         <v>34</v>
       </c>
@@ -8862,8 +9283,11 @@
       <c r="K204" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="205" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L204" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A205" s="5" t="s">
         <v>40</v>
       </c>
@@ -8897,8 +9321,11 @@
       <c r="K205" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="206" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L205" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A206" s="5" t="s">
         <v>45</v>
       </c>
@@ -8932,8 +9359,11 @@
       <c r="K206" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="207" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L206" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A207" s="5" t="s">
         <v>49</v>
       </c>
@@ -8967,8 +9397,11 @@
       <c r="K207" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="208" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L207" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A208" s="5" t="s">
         <v>52</v>
       </c>
@@ -9002,8 +9435,11 @@
       <c r="K208" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="209" spans="1:11" ht="132.6" x14ac:dyDescent="0.3">
+      <c r="L208" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A209" s="5" t="s">
         <v>56</v>
       </c>
@@ -9037,8 +9473,11 @@
       <c r="K209" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="210" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L209" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A210" s="5" t="s">
         <v>61</v>
       </c>
@@ -9072,8 +9511,11 @@
       <c r="K210" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="211" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L210" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A211" s="5" t="s">
         <v>66</v>
       </c>
@@ -9107,8 +9549,11 @@
       <c r="K211" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="212" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L211" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A212" s="5" t="s">
         <v>72</v>
       </c>
@@ -9142,8 +9587,11 @@
       <c r="K212" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="213" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L212" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A213" s="5" t="s">
         <v>78</v>
       </c>
@@ -9177,8 +9625,11 @@
       <c r="K213" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="214" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L213" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
         <v>82</v>
       </c>
@@ -9212,8 +9663,11 @@
       <c r="K214" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="215" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L214" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A215" s="5" t="s">
         <v>85</v>
       </c>
@@ -9247,8 +9701,11 @@
       <c r="K215" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="216" spans="1:11" ht="71.400000000000006" x14ac:dyDescent="0.3">
+      <c r="L215" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12" ht="71.400000000000006" x14ac:dyDescent="0.3">
       <c r="A216" s="5" t="s">
         <v>90</v>
       </c>
@@ -9282,8 +9739,11 @@
       <c r="K216" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="217" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L216" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A217" s="5" t="s">
         <v>93</v>
       </c>
@@ -9317,8 +9777,11 @@
       <c r="K217" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="218" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L217" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A218" s="5" t="s">
         <v>100</v>
       </c>
@@ -9352,8 +9815,11 @@
       <c r="K218" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="219" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L218" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A219" s="5" t="s">
         <v>103</v>
       </c>
@@ -9387,8 +9853,11 @@
       <c r="K219" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="220" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L219" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A220" s="5" t="s">
         <v>109</v>
       </c>
@@ -9422,8 +9891,11 @@
       <c r="K220" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="221" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L220" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A221" s="5" t="s">
         <v>112</v>
       </c>
@@ -9457,8 +9929,11 @@
       <c r="K221" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="222" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L221" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A222" s="5" t="s">
         <v>117</v>
       </c>
@@ -9492,8 +9967,11 @@
       <c r="K222" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="223" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L222" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A223" s="5" t="s">
         <v>123</v>
       </c>
@@ -9527,8 +10005,11 @@
       <c r="K223" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="224" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L223" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A224" s="5" t="s">
         <v>126</v>
       </c>
@@ -9562,8 +10043,11 @@
       <c r="K224" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="225" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L224" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A225" s="5" t="s">
         <v>132</v>
       </c>
@@ -9597,8 +10081,11 @@
       <c r="K225" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="226" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L225" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A226" s="5" t="s">
         <v>137</v>
       </c>
@@ -9632,8 +10119,11 @@
       <c r="K226" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="227" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L226" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A227" s="5" t="s">
         <v>141</v>
       </c>
@@ -9667,8 +10157,11 @@
       <c r="K227" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="228" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L227" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A228" s="5" t="s">
         <v>145</v>
       </c>
@@ -9702,8 +10195,11 @@
       <c r="K228" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="229" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L228" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A229" s="5" t="s">
         <v>151</v>
       </c>
@@ -9737,8 +10233,11 @@
       <c r="K229" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="230" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L229" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A230" s="5" t="s">
         <v>153</v>
       </c>
@@ -9772,8 +10271,11 @@
       <c r="K230" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="231" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L230" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A231" s="5" t="s">
         <v>156</v>
       </c>
@@ -9807,8 +10309,11 @@
       <c r="K231" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="232" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L231" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A232" s="5" t="s">
         <v>162</v>
       </c>
@@ -9842,8 +10347,11 @@
       <c r="K232" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="233" spans="1:11" ht="71.400000000000006" x14ac:dyDescent="0.3">
+      <c r="L232" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12" ht="71.400000000000006" x14ac:dyDescent="0.3">
       <c r="A233" s="5" t="s">
         <v>165</v>
       </c>
@@ -9877,8 +10385,11 @@
       <c r="K233" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="234" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L233" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A234" s="5" t="s">
         <v>171</v>
       </c>
@@ -9912,8 +10423,11 @@
       <c r="K234" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="235" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L234" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A235" s="5" t="s">
         <v>175</v>
       </c>
@@ -9947,8 +10461,11 @@
       <c r="K235" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="236" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L235" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A236" s="5" t="s">
         <v>182</v>
       </c>
@@ -9982,8 +10499,11 @@
       <c r="K236" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="237" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L236" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A237" s="5" t="s">
         <v>182</v>
       </c>
@@ -10017,8 +10537,11 @@
       <c r="K237" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="238" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L237" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A238" s="5" t="s">
         <v>189</v>
       </c>
@@ -10052,8 +10575,11 @@
       <c r="K238" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="239" spans="1:11" ht="91.8" x14ac:dyDescent="0.3">
+      <c r="L238" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A239" s="5" t="s">
         <v>193</v>
       </c>
@@ -10087,8 +10613,11 @@
       <c r="K239" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="240" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L239" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A240" s="5" t="s">
         <v>196</v>
       </c>
@@ -10122,8 +10651,11 @@
       <c r="K240" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="241" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L240" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A241" s="5" t="s">
         <v>199</v>
       </c>
@@ -10157,8 +10689,11 @@
       <c r="K241" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="242" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L241" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A242" s="5" t="s">
         <v>203</v>
       </c>
@@ -10192,8 +10727,11 @@
       <c r="K242" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="243" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L242" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A243" s="5" t="s">
         <v>207</v>
       </c>
@@ -10227,8 +10765,11 @@
       <c r="K243" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="244" spans="1:11" ht="91.8" x14ac:dyDescent="0.3">
+      <c r="L243" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A244" s="5" t="s">
         <v>209</v>
       </c>
@@ -10262,8 +10803,11 @@
       <c r="K244" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="245" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L244" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A245" s="5" t="s">
         <v>210</v>
       </c>
@@ -10297,8 +10841,11 @@
       <c r="K245" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="246" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L245" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A246" s="5" t="s">
         <v>212</v>
       </c>
@@ -10332,8 +10879,11 @@
       <c r="K246" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="247" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L246" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A247" s="5" t="s">
         <v>215</v>
       </c>
@@ -10367,8 +10917,11 @@
       <c r="K247" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="248" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L247" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A248" s="5" t="s">
         <v>217</v>
       </c>
@@ -10402,8 +10955,11 @@
       <c r="K248" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="249" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L248" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A249" s="5" t="s">
         <v>218</v>
       </c>
@@ -10437,8 +10993,11 @@
       <c r="K249" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="250" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L249" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A250" s="5" t="s">
         <v>225</v>
       </c>
@@ -10472,8 +11031,11 @@
       <c r="K250" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="251" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L250" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A251" s="5" t="s">
         <v>227</v>
       </c>
@@ -10507,8 +11069,11 @@
       <c r="K251" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="252" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L251" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A252" s="5" t="s">
         <v>232</v>
       </c>
@@ -10542,8 +11107,11 @@
       <c r="K252" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="253" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L252" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A253" s="5" t="s">
         <v>238</v>
       </c>
@@ -10577,8 +11145,11 @@
       <c r="K253" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="254" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L253" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A254" s="5" t="s">
         <v>243</v>
       </c>
@@ -10612,8 +11183,11 @@
       <c r="K254" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="255" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L254" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A255" s="5" t="s">
         <v>249</v>
       </c>
@@ -10647,8 +11221,11 @@
       <c r="K255" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="256" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L255" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A256" s="5" t="s">
         <v>250</v>
       </c>
@@ -10682,8 +11259,11 @@
       <c r="K256" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="257" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L256" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A257" s="5" t="s">
         <v>255</v>
       </c>
@@ -10717,8 +11297,11 @@
       <c r="K257" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="258" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L257" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A258" s="5" t="s">
         <v>260</v>
       </c>
@@ -10752,8 +11335,11 @@
       <c r="K258" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="259" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L258" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A259" s="5" t="s">
         <v>260</v>
       </c>
@@ -10787,8 +11373,11 @@
       <c r="K259" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="260" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L259" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A260" s="5" t="s">
         <v>260</v>
       </c>
@@ -10822,8 +11411,11 @@
       <c r="K260" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="261" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L260" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A261" s="5" t="s">
         <v>267</v>
       </c>
@@ -10857,8 +11449,11 @@
       <c r="K261" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="262" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L261" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A262" s="5" t="s">
         <v>270</v>
       </c>
@@ -10892,8 +11487,11 @@
       <c r="K262" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="263" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L262" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="263" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A263" s="5" t="s">
         <v>274</v>
       </c>
@@ -10927,8 +11525,11 @@
       <c r="K263" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="264" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L263" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="264" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A264" s="5" t="s">
         <v>278</v>
       </c>
@@ -10962,8 +11563,11 @@
       <c r="K264" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="265" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L264" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="265" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A265" s="5" t="s">
         <v>281</v>
       </c>
@@ -10997,8 +11601,11 @@
       <c r="K265" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="266" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L265" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="266" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A266" s="5" t="s">
         <v>285</v>
       </c>
@@ -11032,8 +11639,11 @@
       <c r="K266" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="267" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L266" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="267" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A267" s="5" t="s">
         <v>290</v>
       </c>
@@ -11067,8 +11677,11 @@
       <c r="K267" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="268" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L267" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="268" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A268" s="5" t="s">
         <v>293</v>
       </c>
@@ -11102,8 +11715,11 @@
       <c r="K268" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="269" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L268" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="269" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A269" s="5" t="s">
         <v>298</v>
       </c>
@@ -11137,8 +11753,11 @@
       <c r="K269" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="270" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L269" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="270" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A270" s="5" t="s">
         <v>301</v>
       </c>
@@ -11172,8 +11791,11 @@
       <c r="K270" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="271" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L270" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A271" s="5" t="s">
         <v>307</v>
       </c>
@@ -11207,8 +11829,11 @@
       <c r="K271" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="272" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L271" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="272" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A272" s="5" t="s">
         <v>312</v>
       </c>
@@ -11242,8 +11867,11 @@
       <c r="K272" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="273" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L272" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A273" s="5" t="s">
         <v>316</v>
       </c>
@@ -11277,8 +11905,11 @@
       <c r="K273" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="274" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L273" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A274" s="5" t="s">
         <v>318</v>
       </c>
@@ -11312,8 +11943,11 @@
       <c r="K274" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="275" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L274" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A275" s="5" t="s">
         <v>321</v>
       </c>
@@ -11347,8 +11981,11 @@
       <c r="K275" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="276" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L275" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A276" s="5" t="s">
         <v>325</v>
       </c>
@@ -11382,8 +12019,11 @@
       <c r="K276" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="277" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L276" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A277" s="5" t="s">
         <v>329</v>
       </c>
@@ -11417,8 +12057,11 @@
       <c r="K277" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="278" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L277" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A278" s="5" t="s">
         <v>331</v>
       </c>
@@ -11452,8 +12095,11 @@
       <c r="K278" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="279" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L278" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="279" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A279" s="5" t="s">
         <v>336</v>
       </c>
@@ -11487,8 +12133,11 @@
       <c r="K279" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="280" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L279" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A280" s="5" t="s">
         <v>339</v>
       </c>
@@ -11522,8 +12171,11 @@
       <c r="K280" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="281" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L280" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="281" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A281" s="5" t="s">
         <v>343</v>
       </c>
@@ -11557,8 +12209,11 @@
       <c r="K281" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="282" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L281" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A282" s="5" t="s">
         <v>345</v>
       </c>
@@ -11592,8 +12247,11 @@
       <c r="K282" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="283" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L282" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A283" s="5" t="s">
         <v>347</v>
       </c>
@@ -11627,8 +12285,11 @@
       <c r="K283" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="284" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L283" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A284" s="5" t="s">
         <v>348</v>
       </c>
@@ -11662,8 +12323,11 @@
       <c r="K284" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="285" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L284" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A285" s="5" t="s">
         <v>353</v>
       </c>
@@ -11697,8 +12361,11 @@
       <c r="K285" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="286" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L285" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A286" s="5" t="s">
         <v>355</v>
       </c>
@@ -11732,8 +12399,11 @@
       <c r="K286" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="287" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L286" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="287" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A287" s="5" t="s">
         <v>358</v>
       </c>
@@ -11767,8 +12437,11 @@
       <c r="K287" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="288" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L287" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="288" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A288" s="5" t="s">
         <v>361</v>
       </c>
@@ -11802,8 +12475,11 @@
       <c r="K288" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="289" spans="1:11" ht="81.599999999999994" x14ac:dyDescent="0.3">
+      <c r="L288" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A289" s="5" t="s">
         <v>363</v>
       </c>
@@ -11837,8 +12513,11 @@
       <c r="K289" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="290" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L289" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="290" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A290" s="5" t="s">
         <v>369</v>
       </c>
@@ -11872,8 +12551,11 @@
       <c r="K290" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="291" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L290" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A291" s="5" t="s">
         <v>373</v>
       </c>
@@ -11907,8 +12589,11 @@
       <c r="K291" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="292" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L291" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="292" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A292" s="5" t="s">
         <v>376</v>
       </c>
@@ -11942,8 +12627,11 @@
       <c r="K292" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="293" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L292" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="293" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A293" s="5" t="s">
         <v>379</v>
       </c>
@@ -11977,8 +12665,11 @@
       <c r="K293" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="294" spans="1:11" ht="91.8" x14ac:dyDescent="0.3">
+      <c r="L293" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="294" spans="1:12" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A294" s="5" t="s">
         <v>383</v>
       </c>
@@ -12012,8 +12703,11 @@
       <c r="K294" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="295" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="L294" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="295" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A295" s="5" t="s">
         <v>385</v>
       </c>
@@ -12047,8 +12741,11 @@
       <c r="K295" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="296" spans="1:11" ht="81.599999999999994" x14ac:dyDescent="0.3">
+      <c r="L295" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="296" spans="1:12" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A296" s="5" t="s">
         <v>389</v>
       </c>
@@ -12082,8 +12779,11 @@
       <c r="K296" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="297" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="L296" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="297" spans="1:12" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A297" s="5" t="s">
         <v>394</v>
       </c>
@@ -12117,8 +12817,11 @@
       <c r="K297" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="298" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L297" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="298" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A298" s="5" t="s">
         <v>399</v>
       </c>
@@ -12152,8 +12855,11 @@
       <c r="K298" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="299" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L298" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="299" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A299" s="5" t="s">
         <v>402</v>
       </c>
@@ -12187,8 +12893,11 @@
       <c r="K299" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="300" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L299" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="300" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A300" s="5" t="s">
         <v>408</v>
       </c>
@@ -12222,8 +12931,11 @@
       <c r="K300" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="301" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L300" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="301" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A301" s="5" t="s">
         <v>411</v>
       </c>
@@ -12257,8 +12969,11 @@
       <c r="K301" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="302" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L301" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="302" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A302" s="5" t="s">
         <v>415</v>
       </c>
@@ -12292,8 +13007,11 @@
       <c r="K302" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="303" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L302" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="303" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A303" s="5" t="s">
         <v>418</v>
       </c>
@@ -12327,8 +13045,11 @@
       <c r="K303" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="304" spans="1:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="L303" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="304" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A304" s="5" t="s">
         <v>421</v>
       </c>
@@ -12362,8 +13083,11 @@
       <c r="K304" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="305" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="L304" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="305" spans="1:12" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A305" s="5" t="s">
         <v>425</v>
       </c>
@@ -12397,8 +13121,12 @@
       <c r="K305" s="8">
         <v>1</v>
       </c>
+      <c r="L305" s="9">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>